<commit_message>
hover.py is the board generating file with other supporting files
</commit_message>
<xml_diff>
--- a/Pandemic Game City Locations.xlsx
+++ b/Pandemic Game City Locations.xlsx
@@ -5,27 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Desktop/python programs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Desktop/python programs/github_attempt/Pandemic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BECAED65-E085-1343-8901-3CC2335AFA2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E957DA1-941A-2D48-9585-AA2E8B4921AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28420" windowHeight="16340" activeTab="1" xr2:uid="{3F002B8B-F2DF-FA4B-8128-C562C0C3616A}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28420" windowHeight="16300" activeTab="1" xr2:uid="{3F002B8B-F2DF-FA4B-8128-C562C0C3616A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Longitude and Latitude" sheetId="2" r:id="rId2"/>
     <sheet name="Population" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Longitude and Latitude'!$A$1:$A$55</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Longitude and Latitude'!$B$1:$B$55</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Longitude and Latitude'!$C$1:$C$55</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Longitude and Latitude'!$D$1:$D$55</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Longitude and Latitude'!$D$2:$D$55</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">('Longitude and Latitude'!$A$2:$A$13,'Longitude and Latitude'!$A$16:$A$27,'Longitude and Latitude'!$A$30:$A$41,'Longitude and Latitude'!$A$44:$A$55)</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">('Longitude and Latitude'!$D$2:$D$13,'Longitude and Latitude'!$D$16:$D$27,'Longitude and Latitude'!$D$30:$D$41,'Longitude and Latitude'!$D$44:$D$55)</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1950,6 +1941,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5A90-F946-8116-D04DC208BFA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1964,6 +1960,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5A90-F946-8116-D04DC208BFA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -1978,6 +1979,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5A90-F946-8116-D04DC208BFA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -1992,6 +1998,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5A90-F946-8116-D04DC208BFA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -5746,7 +5757,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>